<commit_message>
Úprava dokumentace + návrh databáze
</commit_message>
<xml_diff>
--- a/Vlček.xlsx
+++ b/Vlček.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WEB\Projekt WEB aplikace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Drive\Škola\web-repozitar\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069D3846-1D9C-444B-B62D-327207FC058C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC765430-880D-43EC-8293-20C7A837EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t xml:space="preserve"> Na úvodní stránku umístěte funkci PHP pro zápis aktuálního data</t>
   </si>
@@ -162,6 +173,33 @@
   </si>
   <si>
     <t>Rehák, Vlček</t>
+  </si>
+  <si>
+    <t>Splněno?</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>Statistika:</t>
+  </si>
+  <si>
+    <t>Celkem úkolů</t>
+  </si>
+  <si>
+    <t>Zbývá úkolů</t>
+  </si>
+  <si>
+    <t>Splněno úkolů</t>
+  </si>
+  <si>
+    <t>Počet bodů</t>
+  </si>
+  <si>
+    <t>Poznámky k úkolu</t>
+  </si>
+  <si>
+    <t>Body</t>
   </si>
 </sst>
 </file>
@@ -219,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -292,11 +330,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -310,23 +368,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -337,6 +424,846 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>Progress</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7707-4B40-A62D-74D73D280634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>List1!$I$4:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Zbývá úkolů</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Splněno úkolů</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$J$4:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7707-4B40-A62D-74D73D280634}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graf 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B819A664-C5D7-427D-8602-485CD93E8754}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,21 +1541,37 @@
     <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="77.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -638,11 +1581,25 @@
       <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3">
+        <f>IF($E3="ano",$B3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3">
+        <f>COUNTIF(E3:E33,"ano")+COUNTIF(E3:E33,"ne")</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -652,11 +1609,25 @@
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F33" si="0">IF($E4="ano",$B4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <f>COUNTIF(E3:E33,"ne")</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -666,11 +1637,25 @@
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIF(E3:E33,"ano")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -680,11 +1665,25 @@
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <f>SUM(F3:F33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -694,11 +1693,18 @@
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -708,11 +1714,18 @@
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -722,11 +1735,18 @@
       <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -736,11 +1756,18 @@
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -751,8 +1778,15 @@
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4">
         <f>SUM(B3:B11)</f>
@@ -760,7 +1794,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -770,11 +1804,18 @@
       <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -784,11 +1825,18 @@
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -798,11 +1846,18 @@
       <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -812,11 +1867,18 @@
       <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -826,11 +1888,18 @@
       <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -840,11 +1909,18 @@
       <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -854,11 +1930,18 @@
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4">
         <f>SUM(B13:B19)</f>
@@ -866,74 +1949,101 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E21" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4">
         <f>SUM(B21:B24)</f>
         <v>7</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -943,11 +2053,18 @@
       <c r="C26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <v>1</v>
@@ -955,11 +2072,18 @@
       <c r="C27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -969,11 +2093,18 @@
       <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -983,11 +2114,18 @@
       <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -997,11 +2135,18 @@
       <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1014,8 +2159,15 @@
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4">
         <f>SUM(B26:B31)</f>
@@ -1023,7 +2175,7 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4">
         <v>2</v>
@@ -1034,22 +2186,29 @@
       <c r="D33" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E33" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="7"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="7"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="6"/>
@@ -1059,7 +2218,23 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E33 E13:E19 E21:E31 E3:E11">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"ano"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33 E13:E19 E21:E31 E3:E11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"ne"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E33 E13:E19 E21:E31 E3:E11" xr:uid="{863E230A-244C-49EC-95DC-36C4C019B116}">
+      <formula1>"ano,ne"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Změna readme + malá úprava tabulky se zadáním
</commit_message>
<xml_diff>
--- a/Vlček.xlsx
+++ b/Vlček.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Drive\Škola\web-repozitar\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC765430-880D-43EC-8293-20C7A837EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA6DA09-FD94-4086-8CC2-1CA61B1FB47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
   <si>
     <t xml:space="preserve"> Na úvodní stránku umístěte funkci PHP pro zápis aktuálního data</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Body</t>
+  </si>
+  <si>
+    <t>WIP úkolů</t>
   </si>
 </sst>
 </file>
@@ -354,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -374,19 +377,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -395,7 +393,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -409,7 +407,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -523,9 +521,34 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-81BA-485E-A71D-BE8670CF9143}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7707-4B40-A62D-74D73D280634}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -540,19 +563,22 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-7707-4B40-A62D-74D73D280634}"/>
+                <c16:uniqueId val="{00000004-81BA-485E-A71D-BE8670CF9143}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>List1!$I$4:$I$5</c:f>
+              <c:f>List1!$I$4:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Zbývá úkolů</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>WIP úkolů</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Splněno úkolů</c:v>
                 </c:pt>
               </c:strCache>
@@ -560,14 +586,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>List1!$J$4:$J$5</c:f>
+              <c:f>List1!$J$4:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1532,7 +1561,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E3" sqref="E3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,11 +1577,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
@@ -1581,10 +1610,10 @@
       <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F3">
@@ -1609,10 +1638,10 @@
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F4">
@@ -1640,7 +1669,7 @@
       <c r="D5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F5">
@@ -1648,10 +1677,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J5">
-        <f>COUNTIF(E3:E33,"ano")</f>
+        <f>COUNTIF(E3:E33,"wip")</f>
         <v>0</v>
       </c>
     </row>
@@ -1668,7 +1697,7 @@
       <c r="D6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F6">
@@ -1676,10 +1705,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6">
-        <f>SUM(F3:F33)</f>
+        <f>COUNTIF(E3:E33,"ano")</f>
         <v>0</v>
       </c>
     </row>
@@ -1696,11 +1725,18 @@
       <c r="D7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7">
+        <f>SUM(F3:F33)</f>
         <v>0</v>
       </c>
     </row>
@@ -1717,7 +1753,7 @@
       <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F8">
@@ -1738,7 +1774,7 @@
       <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F9">
@@ -1759,7 +1795,7 @@
       <c r="D10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F10">
@@ -1778,7 +1814,7 @@
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F11">
@@ -1807,7 +1843,7 @@
       <c r="D13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F13">
@@ -1828,7 +1864,7 @@
       <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F14">
@@ -1849,7 +1885,7 @@
       <c r="D15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F15">
@@ -1870,7 +1906,7 @@
       <c r="D16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F16">
@@ -1891,7 +1927,7 @@
       <c r="D17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F17">
@@ -1912,7 +1948,7 @@
       <c r="D18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F18">
@@ -1933,7 +1969,7 @@
       <c r="D19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F19">
@@ -1962,7 +1998,7 @@
       <c r="D21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F21">
@@ -1983,7 +2019,7 @@
       <c r="D22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F22">
@@ -2004,7 +2040,7 @@
       <c r="D23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F23">
@@ -2025,7 +2061,7 @@
       <c r="D24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F24">
@@ -2040,8 +2076,6 @@
         <v>7</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -2056,7 +2090,7 @@
       <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F26">
@@ -2075,7 +2109,7 @@
       <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F27">
@@ -2096,7 +2130,7 @@
       <c r="D28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F28">
@@ -2117,7 +2151,7 @@
       <c r="D29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F29">
@@ -2138,7 +2172,7 @@
       <c r="D30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F30">
@@ -2159,7 +2193,7 @@
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F31">
@@ -2186,7 +2220,7 @@
       <c r="D33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F33">
@@ -2196,14 +2230,14 @@
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="11"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
@@ -2218,19 +2252,25 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E33 E13:E19 E21:E31 E3:E11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="E13:E19 E21:E31 E33 E3:E11">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"ne"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"ano"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33 E13:E19 E21:E31 E3:E11">
+  <conditionalFormatting sqref="E33 E30:E31 E26:E28 E21:E24 E13:E19 E3:E11">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"ne"</formula>
+      <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E33 E13:E19 E21:E31 E3:E11" xr:uid="{863E230A-244C-49EC-95DC-36C4C019B116}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25" xr:uid="{863E230A-244C-49EC-95DC-36C4C019B116}">
       <formula1>"ano,ne"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E33 E13:E19 E21:E24 E26:E31 E3:E11" xr:uid="{C6291ADF-4A5B-4126-8E02-BC8F625138C4}">
+      <formula1>"ano,WIP,ne"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>

</xml_diff>

<commit_message>
Přidání složky s php + čas na hlavní stránku
Zatím bych pracoval na php a webdesignu v oddělených složkách. PHP nejde zobrazit v .html souborech a webdesign je jednodušší upravovat v .html.
P.S. V tý excel tabulce jdou odškrtávat úkoly, tak tam nějak průběžně zapisujte, ať v tom je pořádek.
</commit_message>
<xml_diff>
--- a/Vlček.xlsx
+++ b/Vlček.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Drive\Škola\web-repozitar\2.RP_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA6DA09-FD94-4086-8CC2-1CA61B1FB47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5152CF7D-C0B3-4ADB-AB66-8B75B4F245F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t xml:space="preserve"> Na úvodní stránku umístěte funkci PHP pro zápis aktuálního data</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>WIP úkolů</t>
+  </si>
+  <si>
+    <t>ano</t>
   </si>
 </sst>
 </file>
@@ -591,13 +594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,7 +1656,7 @@
       </c>
       <c r="J4">
         <f>COUNTIF(E3:E33,"ne")</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1709,7 +1712,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(E3:E33,"ano")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1737,7 +1740,7 @@
       </c>
       <c r="J7">
         <f>SUM(F3:F33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2041,11 +2044,11 @@
         <v>37</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>